<commit_message>
sensitivity verbetering met k factor
</commit_message>
<xml_diff>
--- a/SOFTWARE/Thermal/1D forloops/Sensitivity 2.0/Sensitivity analysis.xlsx
+++ b/SOFTWARE/Thermal/1D forloops/Sensitivity 2.0/Sensitivity analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Lay 1</t>
   </si>
@@ -156,30 +156,9 @@
     <t>2.6924    2.6924    9.9822    0.0254    0.0254</t>
   </si>
   <si>
-    <t>0.2540    0.2540    8.8392    0.0254    0.0254</t>
-  </si>
-  <si>
-    <t>0.2540    0.2540    9.8044    0.0254    0.0254</t>
-  </si>
-  <si>
     <t>No Go</t>
   </si>
   <si>
-    <t>0.2540    0.2540   10.0584    0.0254    0.0254</t>
-  </si>
-  <si>
-    <t>0.2540    0.2540   10.6680    0.0254    0.0254</t>
-  </si>
-  <si>
-    <t>0.2540    0.2540   11.4808    0.0254    0.0254</t>
-  </si>
-  <si>
-    <t>0.2540    0.2540   12.4460    0.0254    0.0254</t>
-  </si>
-  <si>
-    <t>0.2540    0.2540   11.1252    0.0254    0.0254</t>
-  </si>
-  <si>
     <t>m/A</t>
   </si>
   <si>
@@ -196,6 +175,24 @@
   </si>
   <si>
     <t>0.2540    0.2540    2.9464    0.0254    0.0254</t>
+  </si>
+  <si>
+    <t>0.2540    0.2540    6.5532    0.0254    0.0254</t>
+  </si>
+  <si>
+    <t>0.2540    0.2540    7.7724    0.0254    0.0254</t>
+  </si>
+  <si>
+    <t>0.3810    0.3810    7.5184    0.0254    0.0254</t>
+  </si>
+  <si>
+    <t>1.0922    1.0922    7.5692    0.0254    0.0254</t>
+  </si>
+  <si>
+    <t>0.2540    0.2540   15.0876    0.0254    0.0254</t>
+  </si>
+  <si>
+    <t>0.2540    0.2540   15.5956    0.0254    0.0254</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1063,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -1086,7 +1083,7 @@
         <v>246.89080000000001</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1135,7 +1132,7 @@
         <v>247.7509</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1149,7 +1146,7 @@
         <v>244.61779999999999</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1163,7 +1160,7 @@
         <v>242.529</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1173,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,13 +1216,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K2">
         <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1233,13 +1230,13 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K3">
         <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1247,13 +1244,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K4">
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1261,25 +1258,25 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1.7342</v>
+        <v>1.3653999999999999</v>
       </c>
       <c r="C5">
-        <v>327.60000000000002</v>
+        <v>257.93049999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K5">
         <v>15</v>
       </c>
       <c r="L5">
-        <v>1.8794999999999999</v>
+        <v>2.3041999999999998</v>
       </c>
       <c r="M5">
-        <v>355.0455</v>
+        <v>435.27089999999998</v>
       </c>
       <c r="O5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1287,25 +1284,25 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>1.5889</v>
+        <v>1.2313000000000001</v>
       </c>
       <c r="C6">
-        <v>432.15649999999999</v>
+        <v>334.88740000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="K6">
         <v>18</v>
       </c>
       <c r="L6">
-        <v>1.7733000000000001</v>
+        <v>1.5553999999999999</v>
       </c>
       <c r="M6">
-        <v>482.31079999999997</v>
+        <v>423.03750000000002</v>
       </c>
       <c r="O6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1338,94 +1335,58 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
       <c r="K9">
         <v>6</v>
-      </c>
-      <c r="L9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
       <c r="K10">
         <v>9</v>
-      </c>
-      <c r="L10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
       <c r="K11">
         <v>12</v>
-      </c>
-      <c r="L11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15</v>
       </c>
-      <c r="B12">
-        <v>2.1772</v>
-      </c>
-      <c r="C12">
-        <v>411.2801</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
       <c r="K12">
         <v>15</v>
       </c>
       <c r="L12">
-        <v>2.3239999999999998</v>
+        <v>3.1617000000000002</v>
       </c>
       <c r="M12">
-        <v>439.01350000000002</v>
+        <v>597.25720000000001</v>
       </c>
       <c r="O12" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>2.0131000000000001</v>
-      </c>
-      <c r="C13">
-        <v>547.52530000000002</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
       <c r="K13">
         <v>18</v>
       </c>
       <c r="L13">
-        <v>2.2204000000000002</v>
+        <v>3.0752999999999999</v>
       </c>
       <c r="M13">
-        <v>603.8972</v>
+        <v>836.43100000000004</v>
       </c>
       <c r="O13" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>